<commit_message>
Upgrade: Oanda data loading code
</commit_message>
<xml_diff>
--- a/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
+++ b/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wsl\Microservices-Based-Algorithmic-Trading-System\Storage\minio\storage\airflow-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saeed\Google Drive\Business\Repos\Quant-Trading-Infrastructure\Storage\minio\storage\airflow-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D56A7-744C-4A86-8AB6-400D4A3084F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37F0DF7-7711-4F59-868B-C224C747BC4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
     <sheet name="minute" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Tickers</t>
   </si>
@@ -367,77 +368,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833803CE-59C3-4CA2-B52B-89F040AAE3D2}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0228B1C8-4A34-4FE1-A1A7-1E830D2E48F9}">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833803CE-59C3-4CA2-B52B-89F040AAE3D2}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maint: Updated the Dataloading and indicator loading code
</commit_message>
<xml_diff>
--- a/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
+++ b/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saeed\Google Drive\Business\Repos\Quant-Trading-Infrastructure\Storage\minio\storage\airflow-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37F0DF7-7711-4F59-868B-C224C747BC4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B10205C-7CAC-44A4-91B1-9A30244D5EF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="daily" sheetId="1" r:id="rId1"/>
-    <sheet name="minute" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="d" sheetId="1" r:id="rId1"/>
+    <sheet name="m1" sheetId="2" r:id="rId2"/>
+    <sheet name="h1" sheetId="3" r:id="rId3"/>
+    <sheet name="h4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">d!$A$1:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
   <si>
     <t>Tickers</t>
   </si>
@@ -51,6 +55,12 @@
   </si>
   <si>
     <t>USD_JPY</t>
+  </si>
+  <si>
+    <t>USD_CHF</t>
+  </si>
+  <si>
+    <t>USD_CAD</t>
   </si>
 </sst>
 </file>
@@ -92,7 +102,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -368,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,12 +444,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -396,17 +457,51 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:A10" xr:uid="{B5BFC3CE-F1DE-4DE7-A17B-964F08F06D5F}"/>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{833803CE-59C3-4CA2-B52B-89F040AAE3D2}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,32 +513,141 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0228B1C8-4A34-4FE1-A1A7-1E830D2E48F9}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A11:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A10">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551F9C01-4971-4E05-8DE9-17EDEF42A912}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -453,35 +657,13 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A4:A10">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maint: Secmaster and Indicator DB. Tested Dataloading and edge cases
</commit_message>
<xml_diff>
--- a/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
+++ b/Storage/minio/storage/airflow-files/interested_tickers_oanda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saeed\Google Drive\Business\Repos\Quant-Trading-Infrastructure\Storage\minio\storage\airflow-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B10205C-7CAC-44A4-91B1-9A30244D5EF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1273DEFB-B519-4276-9841-93AED27AE4DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="d" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>Tickers</t>
   </si>
@@ -102,7 +102,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -431,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +500,7 @@
   </sheetData>
   <autoFilter ref="A1:A10" xr:uid="{B5BFC3CE-F1DE-4DE7-A17B-964F08F06D5F}"/>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -558,7 +568,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -569,7 +579,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,10 +636,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A11:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A10">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -637,10 +647,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551F9C01-4971-4E05-8DE9-17EDEF42A912}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,16 +662,51 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A4:A10">
+  <conditionalFormatting sqref="A2:A10">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>